<commit_message>
added lonaconing to the workbook
</commit_message>
<xml_diff>
--- a/Municipal_Zoning_Workbook.xlsx
+++ b/Municipal_Zoning_Workbook.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{D5A872AE-5E3E-4D81-99D4-187F6DBA7714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E77B94C6-4AFE-45D4-887E-82C6B0E5B03D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{486F59E6-5163-4D0F-99BE-51D83D0185AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="City of Frederick" sheetId="1" r:id="rId1"/>
+    <sheet name="Town of Lonaconing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Zone</t>
   </si>
@@ -204,6 +205,39 @@
   </si>
   <si>
     <t>The Mixed Use district is intended to provide a planned district that allows for the integration of residential and nonresidential uses, provides for mixed dwelling unit types and housing densities, provides for compatible and complimentary retail, office, and employment uses; provides for greater flexibility than single-use districts through a planned review process that insures safe, efficient, convenient, harmonious groupings of structures, uses, facilities, and support uses; and provides for the appropriate relationships of space, inside and outside buildings. See §417.</t>
+  </si>
+  <si>
+    <t>LDR</t>
+  </si>
+  <si>
+    <t>Town of Lonaconing Planning and Zoning Department</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>The Town Center (TC) Zoning District is comprised of single family detached dwellings, one dwelling unit in combination with permitted commercial use, twin dwelling, two family detached dwelling, townhouse, and multifamily dwelling.</t>
+  </si>
+  <si>
+    <t>Town Center</t>
+  </si>
+  <si>
+    <t>MDR</t>
+  </si>
+  <si>
+    <t>The Medium Density Residential (MDR) Zoning District is comprised of single family detached dwilling, twin dwelling, two family detached dwelling, townhouse, and multifamily dwelling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixed Use </t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>The Mixed Use (MU) Zoning District is any structure or use; however any dwelling units should include a minimum of 500 square feet of indoor floor area per dwelling unit.</t>
+  </si>
+  <si>
+    <t>The Low Density Residential(LDR) Zoning District is primarily comprised of single family detached dwellings. Although twin dwellings (side-by-side dwellings) are permitted in the LDR as well.</t>
   </si>
 </sst>
 </file>
@@ -577,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E7B62E-95DA-4E26-B4B2-FEA2AC52969B}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,4 +892,95 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DA4B25-0DD4-496B-B72F-AD2DB6C07C4D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="171.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added town of thurmont zoning
</commit_message>
<xml_diff>
--- a/Municipal_Zoning_Workbook.xlsx
+++ b/Municipal_Zoning_Workbook.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{486F59E6-5163-4D0F-99BE-51D83D0185AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD68CA54-F501-4893-B401-783F7D270F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="City of Frederick" sheetId="1" r:id="rId1"/>
-    <sheet name="Town of Lonaconing" sheetId="2" r:id="rId2"/>
+    <sheet name="Town of Thurmont" sheetId="3" r:id="rId2"/>
+    <sheet name="Town of Lonaconing" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
   <si>
     <t>Zone</t>
   </si>
@@ -238,16 +239,130 @@
   </si>
   <si>
     <t>The Low Density Residential(LDR) Zoning District is primarily comprised of single family detached dwellings. Although twin dwellings (side-by-side dwellings) are permitted in the LDR as well.</t>
+  </si>
+  <si>
+    <t>Town of Thurmont Planning and Zoning Department</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Open Space</t>
+  </si>
+  <si>
+    <t>The Open Space (OS) District is intended to provide permanent open space for its natural beauty and recreational value. It is also intended to preserve natural resources, prevent erosion, pollution, silting, and safeguard the health, safety, and welfare of persons and property by limiting development in other areas where protection against natural dangers to life and property, or the lack of such protection, would prove costly to members of the community.</t>
+  </si>
+  <si>
+    <t>Agricultural/Preserve</t>
+  </si>
+  <si>
+    <t>ARP</t>
+  </si>
+  <si>
+    <t>The Agricultural/Preserve District is intended to provide for the preservation of productive farming lands and operations. To preserve open space for its natural beauty and recreational and 48 environmental values and allow space for a limited amount of residential development clustered within preserved open spaces.</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
+    <t>The R-1 District is intended to encourage and promote the development of large lot, single family residential neighborhoods free from congestions and conflicting land uses.</t>
+  </si>
+  <si>
+    <t>R-2</t>
+  </si>
+  <si>
+    <t>The R-2 District is intended to provide for single family residential development on small lots where community sewer and water facilities are constructed or programmed.</t>
+  </si>
+  <si>
+    <t>R-3</t>
+  </si>
+  <si>
+    <t>The R-3 District is intended to provide for a greater mix of residential dwelling types on small lots.</t>
+  </si>
+  <si>
+    <t>R-5</t>
+  </si>
+  <si>
+    <t>The R-5 District is intended to provide for attached single family dwellings on small lots, multi-family dwelling structures, and generally, a variety of residential building types and open spaces to create attractive planned communities.</t>
+  </si>
+  <si>
+    <t>Mixed-use Village</t>
+  </si>
+  <si>
+    <t>MXV-1</t>
+  </si>
+  <si>
+    <t>The Mixed-Use Village-1 (MXV-1) District is established to foster a greater opportunity for creative development or redevelopment of vacant and underused lands for a variety of uses traditionally compatible with the small-town character of Thurmont. The District seeks to encourage the following characteristics: Retail shops, offices, residences, civic space located within walking distance of the TB District and commercial activities, traditional site and building designs, residential uses developed as accessory to commercial uses and new residential in conjunction with non-residential development</t>
+  </si>
+  <si>
+    <t>MXV-2</t>
+  </si>
+  <si>
+    <t>The Mixed-Use Village-2 (MXV-2) District is established to foster a greater opportunity for creative development or redevelopment of existing structures for uses traditionally compatible with the small-town character of Thurmont’s Main Street corridor. The MXV-2 District seeks to encourage the following characteristics: small retail shops, office personal services and residences along or near the Main Street corridor and within comfortable walking distance of the TB District and nearby commercial and civic activities, traditional site design and building design, residential uses maintained or established as accessory to commercial activities in the district, the compact development or redevelopment of lands near Thurmont's primary economic development areas (current and planned), physical development characteristics of one and a half to two and a half story structures with commercial uses on the ground floor and residential uses above.</t>
+  </si>
+  <si>
+    <t>Town Business</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>The Town Business (TB) District is intended to serve residential neighborhoods with necessary retail facilities as well as service establishments, professional offices, social, and religious properties. It is also intended for the central business area of the town. Stores and other facilities should be grouped together in small areas and in an attractive, convenient manner with attention paid to the safety of pedestrian travel.</t>
+  </si>
+  <si>
+    <t>General Business</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>The General Business (GB) District is intended to provide the retail, service, and professional activities covered in the TB Zone as well as other, more intensive commercial uses.</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>The Industrial (I) District is intended for the location of commercial and industrial uses of a warehousing, research, and manufacturing nature. The appropriateness of an industry in this district is to be governed by performance standards to maintain high standards of water, air, noise, odor, and aesthetic quality.</t>
+  </si>
+  <si>
+    <t>Office/Industrial</t>
+  </si>
+  <si>
+    <t>OI</t>
+  </si>
+  <si>
+    <t>The Office/ Industrial (OI) District is intended primarily for office and industrial uses which can intrinsically operate, outside of the town’s legacy (I) Industrial Zoning District, harmoniously with surrounding non-industrial uses, being characterized by attractive building architecture, landscaped sites and streetscapes, and the absence of adverse external impacts to adjoining properties, and to encourage the development in Thurmont of enterprises in professional, scientific, technical, engineering, computing, and both advanced and artisan manufacturing.</t>
+  </si>
+  <si>
+    <t>Institutional</t>
+  </si>
+  <si>
+    <t>INST</t>
+  </si>
+  <si>
+    <t>The institutional (INST) district is intended to provide for the preservation of land for uses that provide for the good and welfare of the community and address the community’s needs for centers and operations for government, culture, education, religion, civic engagement, public health, public safety, and similar.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,8 +388,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,7 +730,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,10 +1013,228 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689C95D2-106B-41D4-9286-ED9B025E1245}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20DA4B25-0DD4-496B-B72F-AD2DB6C07C4D}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated municipal zoning workbook
</commit_message>
<xml_diff>
--- a/Municipal_Zoning_Workbook.xlsx
+++ b/Municipal_Zoning_Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E8B709B-7093-42E6-92D8-1867EF89E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{3E8B709B-7093-42E6-92D8-1867EF89E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78D1775-38F7-41AA-8862-3FACABCA3A42}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="City of Frederick" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="City of Brunswick" sheetId="4" r:id="rId3"/>
     <sheet name="Town of Lonaconing" sheetId="2" r:id="rId4"/>
     <sheet name="Town of Middletown" sheetId="5" r:id="rId5"/>
+    <sheet name="Town of Poolesville" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="159">
   <si>
     <t>Zone</t>
   </si>
@@ -469,6 +470,54 @@
   </si>
   <si>
     <t>The town commercial district is intended to provide areas for frequently used retail, service and employment establishments while maintaining the basic character of the area in which they are located.</t>
+  </si>
+  <si>
+    <t>Residential Multi-Family</t>
+  </si>
+  <si>
+    <t>Residential 1/3 Acre Lots</t>
+  </si>
+  <si>
+    <t>Residential ½ Acre Lots</t>
+  </si>
+  <si>
+    <t>Residential ¾ Acre Lots</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>PR MUL</t>
+  </si>
+  <si>
+    <t>R 1/3</t>
+  </si>
+  <si>
+    <t>R ½</t>
+  </si>
+  <si>
+    <t>R ¾</t>
+  </si>
+  <si>
+    <t>Poolesville Planning and Zoning Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential zoning districts are zones that are developed to house individuals and families. The Residential Multi-Family zone is for residential properties containing multiple family dwelling units like townhouses. </t>
+  </si>
+  <si>
+    <t>P COMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential zoning districts are zones that are developed to house individuals and families. The Residential R 1/3 zone is for residential properties at least 1/3 of an acre in size. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential zoning districts are zones that are developed to house individuals and families. The Residential 1/2 zone is for residential properties at least 1/2 an acre in size. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential zoning districts are zones that are developed to house individuals and families. The Residential 3/4 zone is for residential properties at least 3/4 of an acre in size. </t>
+  </si>
+  <si>
+    <t>Commercial zones are for businesses, restaurants, retail stores, convenience stores, entertainment stores, or automobile shops; however, they also support mixed uses or residential projects. The purpose of the commercial zone is to create a vibrant Town center that serves as a destination for residents and visitors to walk, shop, dine, live, and interact. Development and redevelopment projects should be harmonious with and enhance the characteristics of the Town Center.</t>
   </si>
 </sst>
 </file>
@@ -851,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E7B62E-95DA-4E26-B4B2-FEA2AC52969B}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1661,7 +1710,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,4 +1808,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE043791-1C84-4672-9F69-F7A621112F9C}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added city of cumberland
</commit_message>
<xml_diff>
--- a/Municipal_Zoning_Workbook.xlsx
+++ b/Municipal_Zoning_Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{3E8B709B-7093-42E6-92D8-1867EF89E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78D1775-38F7-41AA-8862-3FACABCA3A42}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{3E8B709B-7093-42E6-92D8-1867EF89E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDDF9464-D940-4F24-BBAD-7305047FAD9C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="City of Frederick" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,9 @@
     <sheet name="Town of Lonaconing" sheetId="2" r:id="rId4"/>
     <sheet name="Town of Middletown" sheetId="5" r:id="rId5"/>
     <sheet name="Town of Poolesville" sheetId="6" r:id="rId6"/>
+    <sheet name="City of Cumberland" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="204">
   <si>
     <t>Zone</t>
   </si>
@@ -518,6 +519,141 @@
   </si>
   <si>
     <t>Commercial zones are for businesses, restaurants, retail stores, convenience stores, entertainment stores, or automobile shops; however, they also support mixed uses or residential projects. The purpose of the commercial zone is to create a vibrant Town center that serves as a destination for residents and visitors to walk, shop, dine, live, and interact. Development and redevelopment projects should be harmonious with and enhance the characteristics of the Town Center.</t>
+  </si>
+  <si>
+    <t>Conservation</t>
+  </si>
+  <si>
+    <t>Estate Residential</t>
+  </si>
+  <si>
+    <t>Suburban Residential</t>
+  </si>
+  <si>
+    <t>Urban Residential</t>
+  </si>
+  <si>
+    <t>Local Business</t>
+  </si>
+  <si>
+    <t>Highway Business</t>
+  </si>
+  <si>
+    <t>Central Business District</t>
+  </si>
+  <si>
+    <t>Business Commercial </t>
+  </si>
+  <si>
+    <t>Industrial-General </t>
+  </si>
+  <si>
+    <t>Gateway-Commercial District</t>
+  </si>
+  <si>
+    <t>Gateway-Industrial District</t>
+  </si>
+  <si>
+    <t>Rehabilitation and Redevelopment Floating Zone District</t>
+  </si>
+  <si>
+    <t>Adaptive Reuse Floating Zone</t>
+  </si>
+  <si>
+    <t>Planned Development Floating Zone</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>R-E</t>
+  </si>
+  <si>
+    <t>R-S</t>
+  </si>
+  <si>
+    <t>R-U</t>
+  </si>
+  <si>
+    <t>B-L</t>
+  </si>
+  <si>
+    <t>B-H</t>
+  </si>
+  <si>
+    <t>G-I</t>
+  </si>
+  <si>
+    <t>R-O</t>
+  </si>
+  <si>
+    <t>B-CBD</t>
+  </si>
+  <si>
+    <t>B-C</t>
+  </si>
+  <si>
+    <t>I-G</t>
+  </si>
+  <si>
+    <t>G-C</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>City of Cumberland Planning and Zoning Department</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to regulate areas which, in the interest of the public health, safety, and general welfare of the city are subject to flooding and encroachment which aggravates flood conditions; are part of or protective of the rights-of-way of an interstate highway; or are located and featured in such a way as to, by reason of slope, geologic conditions, or overall natural character, warrant preservation through limited usage.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide for low-density residential and certain other forms of development in predominantly undeveloped areas, in a manner that protects the natural features of the land.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide for the continuation of low density single family development in areas where existing and most recent single family development has occurred, and to stabilize and protect these areas.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide areas for low and medium density urban residential uses, including single-family detached, single-family attached, and multi-family dwellings.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide areas appropriate for the harmonious mixing of residential and non-residential uses, and to provide for higher density residential development in a variety of housing types. Dwelling units/mixed uses are consistent with this purpose.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide areas adjacent to residential districts in which commercial uses are permitted primarily for the convenience shopping, professional service, and personal service needs of the area residents.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide areas along major highways which are most appropriate for the development of businesses principally serving the needs of highway users and transients, with the servicing of resident convenience shoppers as a secondary function.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to define and provide regulations for the central regional and city core of shopping, business, government, and related activities.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to provide opportunities for both business and commercial uses which exhibit similar functions in areas which are existing or potentially suitable for such uses, and to effect a desirable transition between business, commercial, existing residential, and other uses.</t>
+  </si>
+  <si>
+    <t>The purpose of this zoning district is to permit and encourage modern industrial development and to permit limited commercial development.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to permit and encourage a mixture of commercial and residential uses within the North Mechanic Street/North Centre Street corridor. To encourage preservation of the structures and properties that have historically defined the unique aesthetic character of one of the city's primary entry and egress corridors, and to guide future development in a manner consistent with this character, a set of guidelines related to parking, signage, site and architectural design have been developed for this district.</t>
+  </si>
+  <si>
+    <t>The purpose of this district is to permit and encourage a mixture of industrial/commercial and residential uses within the North Mechanic Street/North Centre Street corridor. To encourage preservation of the structures and properties that have historically defined the unique aesthetic character of one of the city's primary entry and egress corridors, and to guide future development in a manner consistent with this character, a set of guidelines related to parking, signage, site and architectural design have been developed for this district.</t>
+  </si>
+  <si>
+    <t>Certain areas of the city contain abandoned structures that were originally used for industrial, warehouse, or other employment purposes but which are now nonconforming in the district in which they are located. These structures are no longer useful and constitute a detriment to the surrounding neighborhoods and could adversely affect the city's taxable assessment base. The purpose of the Rehabilitation and Redevelopment Floating Zone District is to allow and provide incentive for the reuse, rehabilitation, and redevelopment of such structures in a manner that will allow them to be restored to the active tax rolls and inventory of land in the city, while preserving the integrity of the neighborhood in which they are located. Performance standards have been developed to address compatibility of proposed developments with adjacent residential areas.</t>
+  </si>
+  <si>
+    <t>The purpose of this floating zone district is to govern the comprehensive redevelopment and adaptive reuse of large properties (two (2) or more acres in size) containing one (1) or more structures (encompassing fifty thousand (50,000) square feet or more of gross floor area, either individually or in combination), the principal or primary use or operation of which has been discontinued or abandoned and which would require greater land use flexibility to revitalize or redevelop than may be allowed by alternative zoning classifications.</t>
+  </si>
+  <si>
+    <t>The purpose of the PD—Planned Development Floating Zone is to encourage the application of innovative and creative land use designs for residential and mixed use developments. The district is intended to allow the unified planning and development of large tracts of land suitable in location, area, and character for the uses and structures proposed.</t>
   </si>
 </sst>
 </file>
@@ -1814,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE043791-1C84-4672-9F69-F7A621112F9C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,4 +2049,249 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B12319E-7104-469C-99EC-F16BA81C6550}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added myersville to code
</commit_message>
<xml_diff>
--- a/Municipal_Zoning_Workbook.xlsx
+++ b/Municipal_Zoning_Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/055abc5dbe1424b0/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{3E8B709B-7093-42E6-92D8-1867EF89E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDDF9464-D940-4F24-BBAD-7305047FAD9C}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{3E8B709B-7093-42E6-92D8-1867EF89E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CAAA2FB-7BDA-4C60-9EEC-47FADADF17BA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{CA185F06-9CD4-4691-B86E-FBA6669FCB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="City of Frederick" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Town of Middletown" sheetId="5" r:id="rId5"/>
     <sheet name="Town of Poolesville" sheetId="6" r:id="rId6"/>
     <sheet name="City of Cumberland" sheetId="7" r:id="rId7"/>
+    <sheet name="Town of Myersville" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="222">
   <si>
     <t>Zone</t>
   </si>
@@ -654,6 +655,60 @@
   </si>
   <si>
     <t>The purpose of the PD—Planned Development Floating Zone is to encourage the application of innovative and creative land use designs for residential and mixed use developments. The district is intended to allow the unified planning and development of large tracts of land suitable in location, area, and character for the uses and structures proposed.</t>
+  </si>
+  <si>
+    <t>Single-Family Residential</t>
+  </si>
+  <si>
+    <t>Town of Myersville Planning and Zoning Department</t>
+  </si>
+  <si>
+    <t>Single-Family Smart Growth</t>
+  </si>
+  <si>
+    <t>R1-SG</t>
+  </si>
+  <si>
+    <t>The R-1 District is intended to provide an attractive, pleasant living environment at a sufficient density to maintain an adequate standard of physical maintenance and community service. The district encourages compact development and the optimum utilization of land appropriate for residential use by encouraging the use of planned unit development, leaving excessively sloping areas and flood-prone areas open, free of development, and available for recreational use. The district discourages the intrusion of the commercial and industrial uses that have an annoying and deteriorating effect on residential development. The maximum density in the R-1 District shall be two dwelling units per acre.</t>
+  </si>
+  <si>
+    <t>The R1-SG District is intended to provide an attractive, pleasant living environment at a sufficient density to meet the state's smart growth initiatives, while maintaining an adequate standard of physical maintenance and community service. The district encourages compact development and the optimum utilization of land appropriate for residential use by encouraging the use of planned unit development, leaving excessively sloping areas and flood-prone areas open, free of development, and available for recreational use. The district discourages the intrusion of the commercial and industrial uses that have an annoying and deteriorating effect on residential development.</t>
+  </si>
+  <si>
+    <t>Multi-Family Residential</t>
+  </si>
+  <si>
+    <t>The intent of the R-2 District is to provide areas for multifamily development. It is further established to increase the variety of housing types and sizes while continuing to encourage the provision of the basic amenities of an attractive and safe residential environment. The maximum density in the R-2 District shall be eight dwelling units per acre.</t>
+  </si>
+  <si>
+    <t>The General Commercial District is intended to provide a central area for shopping, service, office and entertainment establishments to service the needs of the entire community and the surrounding area. The uses permitted in this district should be of such character as to provide for comparative shopping needs, service and repair needs, specialized commercial activities and those establishments which cater primarily to the motoring public. The location of such areas should be such that stores and commercial activities can be grouped together in an attractive and convenient manner at locations that will not infringe on residential areas. It is also essential that areas for this district have excellent vehicular accessibility on major thoroughfares that service the community and surrounding area.</t>
+  </si>
+  <si>
+    <t>Village Center</t>
+  </si>
+  <si>
+    <t>The Village Center District is intended to provide a central area for frequent shopping, service, and office and entertainment establishments to service the needs of the entire community, while maintaining the basic character of the area in which they are located. The uses permitted in this district should be of such character as to provide for residential living areas, comparative shopping needs, service and repair needs, specialized commercial activities and those establishments which cater primarily to pedestrian traffic. The location of such areas should be such that stores and commercial activities can be grouped together in an attractive and convenient manner. It is essential that areas for this district have excellent accessibility on various types of thoroughfares that service the community and surrounding area.</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
+    <t>Historic Town Center</t>
+  </si>
+  <si>
+    <t>HTC</t>
+  </si>
+  <si>
+    <t>The HTC District is intended to permit planned development in the VC District in order to preserve an aesthetically pleasing appearance in that district, to avoid the creation of nuisance or nuisance-like conditions in that district, to protect the historic character within that district, and to promote reinvestment and revitalization within that district. The establishment and placement of an HTC District should be such that multifamily residential and commercial activities may be grouped together in an attractive and convenient manner, sensitive to the historic character of the surrounding community. The establishment and placement of an HTC District must provide for appropriate pedestrian access routes to allow pedestrian connectivity to desirable services and businesses within that district.</t>
+  </si>
+  <si>
+    <t>Village Industrial</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>It is the intent of the VI District to provide areas for limited industrial purposes that are not significantly objectionable in terms of noise, odor, fumes, etc., to surrounding properties. The regulations that apply within the district are designed to encourage the formation and continuance of a compatible environment for uses generally classified to be light industrial in nature; protect and reserve undeveloped areas that are suitable for such industries; and discourage encroachment by those residential, commercial, or other uses capable of adversely affecting the basic industrial character of the VI District.</t>
   </si>
 </sst>
 </file>
@@ -2055,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B12319E-7104-469C-99EC-F16BA81C6550}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,4 +2349,138 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC84F0F-9FD4-4DE9-9600-515DF817F379}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>